<commit_message>
Login-page is updated with Requisition form....
</commit_message>
<xml_diff>
--- a/Team-3/CompareGenie/UserStories/Compare-genie-UserStories.xlsx
+++ b/Team-3/CompareGenie/UserStories/Compare-genie-UserStories.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="530" yWindow="610" windowWidth="13120" windowHeight="4990"/>
+    <workbookView xWindow="525" yWindow="615" windowWidth="13125" windowHeight="4995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -82,9 +82,6 @@
     <t xml:space="preserve">AS A Buyer I Should be able to view previous comparison history So THAT it helps further comparison. </t>
   </si>
   <si>
-    <t xml:space="preserve">AS A Buyer I Should be able to </t>
-  </si>
-  <si>
     <t>AS A Buyer I Should be able to get unit of measurement to each parameter of an object.</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>AS A Buyer I Should be able to compare products in number of iterations So THAT comparison can be done multiple times using different parameters.</t>
+  </si>
+  <si>
+    <t>AS A Buyer I Should be able to Register to login further So That it helps me in historical comparision.</t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +158,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -188,6 +194,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,11 +407,11 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="138" customWidth="1"/>
   </cols>
@@ -426,7 +433,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
@@ -515,7 +522,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
@@ -539,7 +546,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
@@ -579,7 +586,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
@@ -610,8 +617,8 @@
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>22</v>
+      <c r="C25" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task on Creating request model and enum class.
</commit_message>
<xml_diff>
--- a/Team-3/CompareGenie/UserStories/Compare-genie-UserStories.xlsx
+++ b/Team-3/CompareGenie/UserStories/Compare-genie-UserStories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>SL No</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>AS A Buyer I Should be able to Register to login further So That it helps me in historical comparision.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS A Buyer I should be able to Save the ADD-PRODUCT Details into Draft So THAT I can Continue the interrepted Comparison later. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS A Buyer I Should be able to Clear the all Data which i was entered So THAT I can Start entering agin without any confusions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS A Buyer I should be able to Save the ADD-PRODUCT Details by iterations So THAT I can Continue the interrepted Comparison later. </t>
   </si>
 </sst>
 </file>
@@ -405,10 +414,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -621,6 +630,30 @@
         <v>26</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ux design and wireframes of the project... CompareGenie..!
</commit_message>
<xml_diff>
--- a/Team-3/CompareGenie/UserStories/Compare-genie-UserStories.xlsx
+++ b/Team-3/CompareGenie/UserStories/Compare-genie-UserStories.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>SL No</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">AS A Buyer I should be able to Save the ADD-PRODUCT Details by iterations So THAT I can Continue the interrepted Comparison later. </t>
+  </si>
+  <si>
+    <t>AS A Buyer I should be able to define the motivation of my comparision So THAT I can Able to get the result based on my motivation.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
@@ -654,6 +657,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>